<commit_message>
Added support for spreadsheet documents
</commit_message>
<xml_diff>
--- a/service/import/src/test/resources/test.xlsx
+++ b/service/import/src/test/resources/test.xlsx
@@ -1,43 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sysserve/development/projects/work/instanta-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sysserve/development/projects/personal/moonshot/service/import/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6959430-2522-D945-824B-89C65190DA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065CCA8-DFFD-9F41-AF22-2E1B92091538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C7013F1E-56A0-A447-84F9-2226FDBDC143}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{C7013F1E-56A0-A447-84F9-2226FDBDC143}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>NAME</t>
   </si>
   <si>
     <t>QUANTITY</t>
@@ -418,54 +408,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199DA009-F487-6D4B-9419-96CC072275C2}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2BB924-62BA-024D-A2D3-7A44BD87C3C6}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -483,13 +425,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -497,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -511,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>

</xml_diff>